<commit_message>
Fixed command line typo
</commit_message>
<xml_diff>
--- a/Experiment results.xlsx
+++ b/Experiment results.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nguyenla/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sasha\workspace\Rubik\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9740" yWindow="600" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="9735" yWindow="600" windowWidth="28800" windowHeight="17595" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -121,14 +121,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -140,6 +140,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -410,57 +413,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.83203125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="15.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.625" customWidth="1"/>
     <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.83203125" customWidth="1"/>
+    <col min="12" max="12" width="15.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.875" customWidth="1"/>
     <col min="15" max="15" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" customWidth="1"/>
+    <col min="16" max="16" width="15.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.625" customWidth="1"/>
     <col min="19" max="19" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="N1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="R1" s="2" t="s">
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="R1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -470,7 +473,7 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F2" t="s">
@@ -479,7 +482,7 @@
       <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J2" t="s">
@@ -488,7 +491,7 @@
       <c r="K2" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="N2" t="s">
@@ -497,7 +500,7 @@
       <c r="O2" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="R2" t="s">
@@ -506,11 +509,11 @@
       <c r="S2" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -520,16 +523,16 @@
       <c r="C3">
         <v>6.73</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>81.760000000000005</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>6.14</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>229.18</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>408.28</v>
       </c>
       <c r="J3">
@@ -538,7 +541,7 @@
       <c r="K3">
         <v>1</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="2">
         <v>13</v>
       </c>
       <c r="N3">
@@ -547,7 +550,7 @@
       <c r="O3">
         <v>1</v>
       </c>
-      <c r="P3" s="3">
+      <c r="P3" s="2">
         <v>13</v>
       </c>
       <c r="R3">
@@ -556,11 +559,11 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="T3" s="3">
+      <c r="T3" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -570,16 +573,16 @@
       <c r="C4">
         <v>73.599999999999994</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>884.2</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>5.44</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>191.39</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>377.92</v>
       </c>
       <c r="J4">
@@ -588,7 +591,7 @@
       <c r="K4">
         <v>2.13</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="2">
         <v>23.56</v>
       </c>
       <c r="N4">
@@ -597,7 +600,7 @@
       <c r="O4">
         <v>1.97</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P4" s="2">
         <v>24.64</v>
       </c>
       <c r="R4">
@@ -606,11 +609,11 @@
       <c r="S4">
         <v>2.06</v>
       </c>
-      <c r="T4" s="3">
+      <c r="T4" s="2">
         <v>25.72</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -620,16 +623,16 @@
       <c r="C5">
         <v>781.22</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>9375.64</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>129.62</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>9149.9500000000007</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>9344.56</v>
       </c>
       <c r="J5">
@@ -638,7 +641,7 @@
       <c r="K5">
         <v>3.42</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="2">
         <v>42.04</v>
       </c>
       <c r="N5">
@@ -647,7 +650,7 @@
       <c r="O5">
         <v>3.19</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5" s="2">
         <v>39.28</v>
       </c>
       <c r="R5">
@@ -656,11 +659,11 @@
       <c r="S5">
         <v>3.33</v>
       </c>
-      <c r="T5" s="3">
+      <c r="T5" s="2">
         <v>40.96</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -670,16 +673,16 @@
       <c r="C6">
         <v>8251.5499999999993</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>99019.6</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>116.14</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>8182.66</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>8380</v>
       </c>
       <c r="J6">
@@ -688,7 +691,7 @@
       <c r="K6">
         <v>6.39</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="2">
         <v>77.680000000000007</v>
       </c>
       <c r="N6">
@@ -697,7 +700,7 @@
       <c r="O6">
         <v>5.86</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6" s="2">
         <v>69.16</v>
       </c>
       <c r="R6">
@@ -706,11 +709,11 @@
       <c r="S6">
         <v>6.02</v>
       </c>
-      <c r="T6" s="3">
+      <c r="T6" s="2">
         <v>73.239999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -720,7 +723,7 @@
       <c r="C7">
         <v>94793.47</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>1137522.6399999999</v>
       </c>
       <c r="J7">
@@ -729,7 +732,7 @@
       <c r="K7">
         <v>13.88</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="2">
         <v>167.56</v>
       </c>
       <c r="N7">
@@ -738,7 +741,7 @@
       <c r="O7">
         <v>10.66</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7" s="2">
         <v>128.91999999999999</v>
       </c>
       <c r="R7">
@@ -747,11 +750,11 @@
       <c r="S7">
         <v>16.02</v>
       </c>
-      <c r="T7" s="3">
+      <c r="T7" s="2">
         <v>193.24</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -761,7 +764,7 @@
       <c r="K8">
         <v>64.319999999999993</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="2">
         <v>772.84</v>
       </c>
       <c r="N8">
@@ -770,7 +773,7 @@
       <c r="O8">
         <v>24.73</v>
       </c>
-      <c r="P8" s="3">
+      <c r="P8" s="2">
         <v>297.76</v>
       </c>
       <c r="R8">
@@ -779,11 +782,11 @@
       <c r="S8">
         <v>69.92</v>
       </c>
-      <c r="T8" s="3">
+      <c r="T8" s="2">
         <v>840.04</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -793,7 +796,7 @@
       <c r="K9">
         <v>314.16000000000003</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="2">
         <v>3770.92</v>
       </c>
       <c r="N9">
@@ -802,20 +805,20 @@
       <c r="O9">
         <v>187.37</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9" s="2">
         <v>2249.44</v>
       </c>
       <c r="R9">
-        <v>202.92</v>
+        <v>307.10000000000002</v>
       </c>
       <c r="S9">
-        <v>226.5</v>
-      </c>
-      <c r="T9" s="3">
-        <v>2719</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+        <v>333.19</v>
+      </c>
+      <c r="T9" s="2">
+        <v>3999.28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -825,7 +828,7 @@
       <c r="K10">
         <v>1355.45</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="2">
         <v>16266.4</v>
       </c>
       <c r="N10">
@@ -834,7 +837,7 @@
       <c r="O10">
         <v>587.63</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10" s="2">
         <v>7052.56</v>
       </c>
       <c r="R10">
@@ -843,11 +846,11 @@
       <c r="S10">
         <v>1544.75</v>
       </c>
-      <c r="T10" s="3">
+      <c r="T10" s="2">
         <v>18538</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -857,7 +860,7 @@
       <c r="K11">
         <v>13693.97</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11" s="2">
         <v>164328.64000000001</v>
       </c>
       <c r="N11">
@@ -866,7 +869,7 @@
       <c r="O11">
         <v>2386.06</v>
       </c>
-      <c r="P11" s="3">
+      <c r="P11" s="2">
         <v>28633.72</v>
       </c>
       <c r="R11">
@@ -875,11 +878,11 @@
       <c r="S11">
         <v>12551.24</v>
       </c>
-      <c r="T11" s="3">
+      <c r="T11" s="2">
         <v>150615.88</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -889,7 +892,7 @@
       <c r="K12">
         <v>70497.2</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="2">
         <v>845967.4</v>
       </c>
       <c r="N12">
@@ -898,34 +901,34 @@
       <c r="O12">
         <v>19511.439999999999</v>
       </c>
-      <c r="P12" s="3">
+      <c r="P12" s="2">
         <v>234138.18</v>
       </c>
-      <c r="Q12" s="5"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="Q12" s="4"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="5"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="N19">
         <v>19807.52</v>
       </c>
       <c r="O19">
         <v>22545.24</v>
       </c>
-      <c r="P19" s="3">
+      <c r="P19" s="2">
         <v>270543.78000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>